<commit_message>
Další způsob regulace (ten v CA modelu)
</commit_message>
<xml_diff>
--- a/regulace/regulace.xlsx
+++ b/regulace/regulace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FIT\SIM\IMS\regulace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD70722-3E5F-4847-B3AE-81CC03010FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD9315E-7889-4FB2-9588-49361A08748B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1596" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>https://www.obnovitelne.cz/cz/clanek/916/hrabos-se-neda-porazit-muzeme-jen-udrzet-jeho-populaci-v-unosnych-mezich/</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>predátoři</t>
+  </si>
+  <si>
+    <t>Zmenšením výměr polí a obnovením mezí, remízků a jakýchkoliv trvalých porostů zvyšujících diverzitu krajiny by se rovnováha mezi predátorem a kořistí lépe vyrovnávala a fungovala jako trvalá ochrana. </t>
+  </si>
+  <si>
+    <t>zmenšení výměry polí, remízky</t>
   </si>
 </sst>
 </file>
@@ -390,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,9 +441,19 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -445,6 +461,6 @@
     <hyperlink ref="A1" r:id="rId1" xr:uid="{DFA6C4FC-7D15-46F1-8CE9-E6DE811D28BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>